<commit_message>
Buoy and sports data cleaned & joined
</commit_message>
<xml_diff>
--- a/BasketballData_1014.xlsx
+++ b/BasketballData_1014.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="1760" windowWidth="28800" windowHeight="17620" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="3160" yWindow="1760" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="2012ATTD" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="461">
   <si>
     <t>YEAR</t>
   </si>
@@ -1415,9 +1415,6 @@
   </si>
   <si>
     <t>53-29</t>
-  </si>
-  <si>
-    <t>Tue, Apr 16</t>
   </si>
 </sst>
 </file>
@@ -1428,7 +1425,7 @@
     <numFmt numFmtId="164" formatCode="ddd\,\ mmm\ d"/>
     <numFmt numFmtId="165" formatCode="d\-m"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1438,15 +1435,18 @@
       <sz val="11"/>
       <color rgb="FF6C6D6F"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF6C6D6F"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1461,24 +1461,29 @@
     <font>
       <sz val="9"/>
       <name val="Helvetica"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Helvetica"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1490,6 +1495,7 @@
       <sz val="11"/>
       <color rgb="FFCC0000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -1504,6 +1510,7 @@
       <sz val="11"/>
       <color rgb="FF009444"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1514,6 +1521,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -1525,6 +1533,8 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -1537,12 +1547,6 @@
       <sz val="9"/>
       <color rgb="FFCC0000"/>
       <name val="-apple-system"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF6C6D6F"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1580,7 +1584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1708,7 +1712,6 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1989,10 +1992,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F406"/>
+  <dimension ref="A1:F405"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2817,17 +2820,7 @@
         <v>18624</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="16">
-        <v>2013</v>
-      </c>
-      <c r="B42" s="49" t="s">
-        <v>461</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>15</v>
-      </c>
-    </row>
+    <row r="42" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
     <row r="43" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
     <row r="44" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
     <row r="45" spans="1:6" ht="13" x14ac:dyDescent="0.15"/>
@@ -3191,7 +3184,6 @@
     <row r="403" ht="13" x14ac:dyDescent="0.15"/>
     <row r="404" ht="13" x14ac:dyDescent="0.15"/>
     <row r="405" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="406" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
@@ -5914,7 +5906,7 @@
   </sheetPr>
   <dimension ref="A1:F999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>

</xml_diff>